<commit_message>
ongoing testing work ... ongoing Repo tests
</commit_message>
<xml_diff>
--- a/test/RepoTests/ColorsRepo.Tests/TestJson.xlsx
+++ b/test/RepoTests/ColorsRepo.Tests/TestJson.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MitchellDenC\source\repos\EDennis.AspNetCore.Base\test\RepoTests\RepoTests\ColorsRepo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denmi\source\repos\EDennis.AspNetCore.Base\test\RepoTests\ColorsRepo.Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBF694F-B959-4DE2-88DC-7CEDB8F045F9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6D65AB-518B-47E6-A21B-0997176CFCC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="255" windowWidth="25440" windowHeight="15390" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
+    <workbookView xWindow="345" yWindow="0" windowWidth="17993" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,13 +96,6 @@
     <t>Delete</t>
   </si>
   <si>
-    <t>[		   
-  {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},
-  {"Id":-999005,"SysStart":"2018-05-05","Name":"green","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},		    
-  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"}		
-]</t>
-  </si>
-  <si>
     <t>{"Id":-999007,"Name":"violet"}</t>
   </si>
   <si>
@@ -122,14 +115,29 @@
 ]</t>
   </si>
   <si>
+    <t>ReadSeedHistory</t>
+  </si>
+  <si>
+    <t>[
+  {"Id":-999002,"SysStart":"2017-02-02","Name":"pearl","SysEnd":"2018-02-01 23:59:59.9999999","SysUser":"jill@hill.org","SysUserNext":"jack@hill.org"}		    
+]</t>
+  </si>
+  <si>
+    <t>[		   
+  {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
+  {"Id":-999005,"SysStart":"2018-05-05","Name":"green","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},		    
+  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}		
+]</t>
+  </si>
+  <si>
     <t>[
   {"Id":-999001,"SysStart":"2018-01-01","Name":"black","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},
   {"Id":-999002,"SysStart":"2018-02-02","Name":"white","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		    
   {"Id":-999003,"SysStart":"2018-03-03","Name":"gray","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		   
-  {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},
-  {"Id":-999005,"SysStart":"2018-05-05","Name":"green","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},		    
-  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},
-  {"Id":-999007,"SysStart":"2020-01-01","Name":"violet","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"}
+  {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
+  {"Id":-999005,"SysStart":"2018-05-05","Name":"green","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},		    
+  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
+  {"Id":-999007,"SysStart":"2020-01-01","Name":"violet","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
 ]</t>
   </si>
   <si>
@@ -137,10 +145,10 @@
   {"Id":-999001,"SysStart":"2018-01-01","Name":"black","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},
   {"Id":-999002,"SysStart":"2018-02-02","Name":"white","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		    
   {"Id":-999003,"SysStart":"2018-03-03","Name":"gray","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		   
-  {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},
-  {"Id":-999005,"SysStart":"2018-05-05","Name":"green","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},		    
-  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},
-  {"Id":-999007,"SysStart":"2020-01-01","Name":"brown","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"}
+  {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
+  {"Id":-999005,"SysStart":"2018-05-05","Name":"green","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},		    
+  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
+  {"Id":-999007,"SysStart":"2020-01-01","Name":"brown","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
 ]</t>
   </si>
   <si>
@@ -148,10 +156,16 @@
   {"Id":-999001,"SysStart":"2018-01-01","Name":"black","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},
   {"Id":-999002,"SysStart":"2018-02-02","Name":"white","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		    
   {"Id":-999003,"SysStart":"2018-03-03","Name":"gray","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		   
-  {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},
-  {"Id":-999005,"SysStart":"2020-01-01","Name":"olive","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},		    
-  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},
-  {"Id":-999007,"SysStart":"2018-07-07","Name":"violet","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"}
+  {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
+  {"Id":-999005,"SysStart":"2020-01-01","Name":"olive","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},		    
+  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
+  {"Id":-999007,"SysStart":"2018-07-07","Name":"violet","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
+]</t>
+  </si>
+  <si>
+    <t>[
+  {"Id":-999002,"SysStart":"2017-02-02","Name":"pearl","SysEnd":"2018-02-01 23:59:59.9999999","SysUser":"jill@hill.org","SysUserNext":"jack@hill.org"},  
+  {"Id":-999005,"SysStart":"2018-05-05","Name":"green","SysEnd":"2020-01-01","SysUser":"tester@example.org","SysUserNext":"tester@example.org"}		    
 ]</t>
   </si>
   <si>
@@ -159,10 +173,16 @@
   {"Id":-999001,"SysStart":"2018-01-01","Name":"black","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},
   {"Id":-999002,"SysStart":"2018-02-02","Name":"white","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		    
   {"Id":-999003,"SysStart":"2018-03-03","Name":"gray","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		   
-  {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},
-  {"Id":-999005,"SysStart":"2018-05-05","Name":"olive","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},		    
-  {"Id":-999006,"SysStart":"2020-01-01","Name":"indigo","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},
-  {"Id":-999007,"SysStart":"2018-07-07","Name":"violet","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"}
+  {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
+  {"Id":-999005,"SysStart":"2018-05-05","Name":"olive","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},		    
+  {"Id":-999006,"SysStart":"2020-01-01","Name":"indigo","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
+  {"Id":-999007,"SysStart":"2018-07-07","Name":"violet","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
+]</t>
+  </si>
+  <si>
+    <t>[
+  {"Id":-999002,"SysStart":"2017-02-02","Name":"pearl","SysEnd":"2018-02-01 23:59:59.9999999","SysUser":"jill@hill.org","SysUserNext":"jack@hill.org"},  
+  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"2020-01-01","SysUser":"tester@example.org","SysUserNext":"tester@example.org"}		    
 ]</t>
   </si>
   <si>
@@ -170,9 +190,9 @@
   {"Id":-999001,"SysStart":"2018-01-01","Name":"black","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},
   {"Id":-999002,"SysStart":"2018-02-02","Name":"white","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		    
   {"Id":-999003,"SysStart":"2018-03-03","Name":"gray","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		   
-  {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},
-  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},
-  {"Id":-999007,"SysStart":"2018-07-07","Name":"violet","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"}
+  {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
+  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
+  {"Id":-999007,"SysStart":"2018-07-07","Name":"violet","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
 ]</t>
   </si>
   <si>
@@ -180,29 +200,9 @@
   {"Id":-999001,"SysStart":"2018-01-01","Name":"black","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},
   {"Id":-999002,"SysStart":"2018-02-02","Name":"white","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		    
   {"Id":-999003,"SysStart":"2018-03-03","Name":"gray","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		   
-  {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},
-  {"Id":-999005,"SysStart":"2018-05-05","Name":"olive","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"},		    
-  {"Id":-999007,"SysStart":"2018-07-07","Name":"violet","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"testuser@example.org"}
-]</t>
-  </si>
-  <si>
-    <t>ReadSeedHistory</t>
-  </si>
-  <si>
-    <t>[
-  {"Id":-999002,"SysStart":"2017-02-02","Name":"pearl","SysEnd":"2018-02-01 23:59:59.9999999","SysUser":"jill@hill.org","SysUserNext":"jack@hill.org"}		    
-]</t>
-  </si>
-  <si>
-    <t>[
-  {"Id":-999002,"SysStart":"2017-02-02","Name":"pearl","SysEnd":"2018-02-01 23:59:59.9999999","SysUser":"jill@hill.org","SysUserNext":"jack@hill.org"},  
-  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"2020-01-01","SysUser":"testuser@example.org","SysUserNext":"testuser@example.org"}		    
-]</t>
-  </si>
-  <si>
-    <t>[
-  {"Id":-999002,"SysStart":"2017-02-02","Name":"pearl","SysEnd":"2018-02-01 23:59:59.9999999","SysUser":"jill@hill.org","SysUserNext":"jack@hill.org"},  
-  {"Id":-999005,"SysStart":"2018-05-05","Name":"green","SysEnd":"2020-01-01","SysUser":"testuser@example.org","SysUserNext":"testuser@example.org"}		    
+  {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
+  {"Id":-999005,"SysStart":"2018-05-05","Name":"olive","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},		    
+  {"Id":-999007,"SysStart":"2018-07-07","Name":"violet","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
 ]</t>
   </si>
 </sst>
@@ -582,22 +582,22 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.59765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.73046875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1328125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="79.85546875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="79.86328125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -620,7 +620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -640,10 +640,10 @@
         <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -663,10 +663,10 @@
         <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -683,13 +683,13 @@
         <v>11</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -706,10 +706,10 @@
         <v>15</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -726,10 +726,10 @@
         <v>16</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -746,10 +746,10 @@
         <v>15</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -766,10 +766,10 @@
         <v>16</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -786,10 +786,10 @@
         <v>15</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -806,10 +806,10 @@
         <v>16</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -826,10 +826,10 @@
         <v>18</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -846,10 +846,10 @@
         <v>15</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
@@ -866,10 +866,10 @@
         <v>16</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
@@ -886,10 +886,10 @@
         <v>18</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
@@ -909,7 +909,7 @@
         <v>-999005</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
@@ -926,10 +926,10 @@
         <v>16</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>9</v>
       </c>
@@ -946,10 +946,10 @@
         <v>18</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
@@ -969,7 +969,7 @@
         <v>-999006</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
         <v>9</v>
       </c>
@@ -986,10 +986,10 @@
         <v>16</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
         <v>9</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>18</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revised GetPrimaryKeyPredicate in TemporalRepo -- so that it does not require presence of corresponding TEntity instance in current table
</commit_message>
<xml_diff>
--- a/test/RepoTests/ColorsRepo.Tests/TestJson.xlsx
+++ b/test/RepoTests/ColorsRepo.Tests/TestJson.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denmi\source\repos\EDennis.AspNetCore.Base\test\RepoTests\ColorsRepo.Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6D65AB-518B-47E6-A21B-0997176CFCC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA665D2-6AE5-471B-82AB-CFE9F1545017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="0" windowWidth="17993" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
@@ -191,8 +191,7 @@
   {"Id":-999002,"SysStart":"2018-02-02","Name":"white","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		    
   {"Id":-999003,"SysStart":"2018-03-03","Name":"gray","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		   
   {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
-  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
-  {"Id":-999007,"SysStart":"2018-07-07","Name":"violet","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
+  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
 ]</t>
   </si>
   <si>
@@ -201,8 +200,7 @@
   {"Id":-999002,"SysStart":"2018-02-02","Name":"white","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		    
   {"Id":-999003,"SysStart":"2018-03-03","Name":"gray","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		   
   {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
-  {"Id":-999005,"SysStart":"2018-05-05","Name":"olive","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},		    
-  {"Id":-999007,"SysStart":"2018-07-07","Name":"violet","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
+  {"Id":-999005,"SysStart":"2018-05-05","Name":"olive","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
 ]</t>
   </si>
 </sst>
@@ -581,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DF70F6-41B8-4967-A575-80BF52770920}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="C18" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -917,7 +915,7 @@
         <v>10</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>7</v>
@@ -937,7 +935,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>7</v>
@@ -977,7 +975,7 @@
         <v>10</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>8</v>
@@ -997,7 +995,7 @@
         <v>10</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
ColorsRepoTests (TemporalRepo tests) now passing
</commit_message>
<xml_diff>
--- a/test/RepoTests/ColorsRepo.Tests/TestJson.xlsx
+++ b/test/RepoTests/ColorsRepo.Tests/TestJson.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denmi\source\repos\EDennis.AspNetCore.Base\test\RepoTests\ColorsRepo.Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA665D2-6AE5-471B-82AB-CFE9F1545017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF929E5-7899-434D-83E9-F9919A8F8195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="0" windowWidth="17993" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
+    <workbookView xWindow="743" yWindow="608" windowWidth="18397" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="39">
   <si>
     <t>ProjectName</t>
   </si>
@@ -157,15 +157,7 @@
   {"Id":-999002,"SysStart":"2018-02-02","Name":"white","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		    
   {"Id":-999003,"SysStart":"2018-03-03","Name":"gray","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		   
   {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
-  {"Id":-999005,"SysStart":"2020-01-01","Name":"olive","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},		    
-  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
-  {"Id":-999007,"SysStart":"2018-07-07","Name":"violet","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
-]</t>
-  </si>
-  <si>
-    <t>[
-  {"Id":-999002,"SysStart":"2017-02-02","Name":"pearl","SysEnd":"2018-02-01 23:59:59.9999999","SysUser":"jill@hill.org","SysUserNext":"jack@hill.org"},  
-  {"Id":-999005,"SysStart":"2018-05-05","Name":"green","SysEnd":"2020-01-01","SysUser":"tester@example.org","SysUserNext":"tester@example.org"}		    
+  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
 ]</t>
   </si>
   <si>
@@ -174,15 +166,8 @@
   {"Id":-999002,"SysStart":"2018-02-02","Name":"white","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		    
   {"Id":-999003,"SysStart":"2018-03-03","Name":"gray","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		   
   {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
-  {"Id":-999005,"SysStart":"2018-05-05","Name":"olive","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},		    
-  {"Id":-999006,"SysStart":"2020-01-01","Name":"indigo","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
-  {"Id":-999007,"SysStart":"2018-07-07","Name":"violet","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
-]</t>
-  </si>
-  <si>
-    <t>[
-  {"Id":-999002,"SysStart":"2017-02-02","Name":"pearl","SysEnd":"2018-02-01 23:59:59.9999999","SysUser":"jill@hill.org","SysUserNext":"jack@hill.org"},  
-  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"2020-01-01","SysUser":"tester@example.org","SysUserNext":"tester@example.org"}		    
+  {"Id":-999005,"SysStart":"2020-01-01","Name":"olive","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},		    
+  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
 ]</t>
   </si>
   <si>
@@ -191,7 +176,17 @@
   {"Id":-999002,"SysStart":"2018-02-02","Name":"white","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		    
   {"Id":-999003,"SysStart":"2018-03-03","Name":"gray","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		   
   {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
-  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
+  {"Id":-999005,"SysStart":"2018-05-05","Name":"green","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
+]</t>
+  </si>
+  <si>
+    <t>[
+  {"Id":-999005,"SysStart":"2018-05-05","Name":"green","SysEnd":"2020-01-01","SysUser":"tester@example.org","SysUserNext":"tester@example.org"}
+]</t>
+  </si>
+  <si>
+    <t>[
+  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"2020-01-01","SysUser":"tester@example.org","SysUserNext":"tester@example.org"}
 ]</t>
   </si>
   <si>
@@ -200,7 +195,20 @@
   {"Id":-999002,"SysStart":"2018-02-02","Name":"white","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		    
   {"Id":-999003,"SysStart":"2018-03-03","Name":"gray","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"jack@hill.org"},		   
   {"Id":-999004,"SysStart":"2018-04-04","Name":"red","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},
-  {"Id":-999005,"SysStart":"2018-05-05","Name":"olive","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
+  {"Id":-999005,"SysStart":"2018-05-05","Name":"green","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"},		       
+  {"Id":-999006,"SysStart":"2020-01-01","Name":"indigo","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
+]</t>
+  </si>
+  <si>
+    <t>[
+  {"Id":-999006,"SysStart":"2018-06-06","Name":"blue","SysEnd":"2020-01-01","SysUser":"tester@example.org","SysUserNext":"tester@example.org"},
+  {"Id":-999006,"SysStart":"2020-01-01","Name":"indigo","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
+]</t>
+  </si>
+  <si>
+    <t>[
+  {"Id":-999005,"SysStart":"2018-05-05","Name":"green","SysEnd":"2020-01-01","SysUser":"tester@example.org","SysUserNext":"tester@example.org"},
+  {"Id":-999005,"SysStart":"2020-01-01","Name":"olive","SysEnd":"9999-12-31 23:59:59.9999999","SysUser":"tester@example.org"}
 ]</t>
   </si>
 </sst>
@@ -577,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DF70F6-41B8-4967-A575-80BF52770920}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C18" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -787,7 +795,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -801,13 +809,13 @@
         <v>7</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+      <c r="G10" s="3">
+        <v>-999005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -821,13 +829,13 @@
         <v>7</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -838,16 +846,16 @@
         <v>17</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
@@ -861,13 +869,13 @@
         <v>8</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
@@ -881,53 +889,53 @@
         <v>8</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="3">
+        <v>-999006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="3">
-        <v>-999005</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="G16" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>9</v>
       </c>
@@ -941,13 +949,13 @@
         <v>7</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+      <c r="G17" s="3">
+        <v>-999005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
@@ -958,16 +966,16 @@
         <v>20</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="3">
-        <v>-999006</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
         <v>9</v>
       </c>
@@ -978,16 +986,16 @@
         <v>20</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
         <v>9</v>
       </c>
@@ -1001,10 +1009,50 @@
         <v>8</v>
       </c>
       <c r="F20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="3">
+        <v>-999006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>34</v>
+      <c r="G22" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>